<commit_message>
code to connect all the necessary nodes in accordance with excel data
</commit_message>
<xml_diff>
--- a/servers-test-upload.xlsx
+++ b/servers-test-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joseph\CAD\Semseter 2\System Development Project\test-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F920022-0217-402F-9F46-48EBB6CD9E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF37818-9142-4C91-AE43-3B4B6831CEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>IP</t>
+  </si>
+  <si>
+    <t>ConnectsTo</t>
+  </si>
+  <si>
+    <t>Server3, Server4</t>
   </si>
 </sst>
 </file>
@@ -104,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -112,6 +118,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -401,41 +408,54 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -443,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
nodes and links wiht boundaries. Working model
</commit_message>
<xml_diff>
--- a/servers-test-upload.xlsx
+++ b/servers-test-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joseph\CAD\Semseter 2\System Development Project\test-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF37818-9142-4C91-AE43-3B4B6831CEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC369895-4DEA-4E95-89DC-41AD67F28F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -66,7 +66,25 @@
     <t>ConnectsTo</t>
   </si>
   <si>
-    <t>Server3, Server4</t>
+    <t>Firewall1</t>
+  </si>
+  <si>
+    <t>Firewall2</t>
+  </si>
+  <si>
+    <t>Firewall3</t>
+  </si>
+  <si>
+    <t>192.168.6.1</t>
+  </si>
+  <si>
+    <t>192.168.8.1</t>
+  </si>
+  <si>
+    <t>192.168.7.1</t>
+  </si>
+  <si>
+    <t>Server3, Firewall2</t>
   </si>
 </sst>
 </file>
@@ -399,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -441,7 +459,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -452,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -463,12 +481,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
label with node name and ip address
</commit_message>
<xml_diff>
--- a/servers-test-upload.xlsx
+++ b/servers-test-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joseph\CAD\Semseter 2\System Development Project\test-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC369895-4DEA-4E95-89DC-41AD67F28F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECB812F-58D0-4AAC-A64D-42490F54E8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Server3, Firewall2</t>
+  </si>
+  <si>
+    <t>Server6</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,6 +525,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaned code for Iteration 1 final
</commit_message>
<xml_diff>
--- a/servers-test-upload.xlsx
+++ b/servers-test-upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joseph\CAD\Semseter 2\System Development Project\test-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECB812F-58D0-4AAC-A64D-42490F54E8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E92FA6-21E3-45F4-A236-43A1A23E79E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Server6</t>
+  </si>
+  <si>
+    <t>Server 7</t>
+  </si>
+  <si>
+    <t>192.168.9.1</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,6 +542,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>